<commit_message>
Update Liz example data
</commit_message>
<xml_diff>
--- a/inst/extdata/exampleGosling_2020.xlsx
+++ b/inst/extdata/exampleGosling_2020.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20370"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\X\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\GIT\optimlanduse\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{269DBBA6-B99D-4A8E-89E8-EC9D93F575D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3039ED6A-B6C0-41D0-B2BE-A93F5FF2AF6A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{3D0FC10B-2B2D-436E-AC0A-EC57326BA3DE}"/>
   </bookViews>
@@ -98,7 +98,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -294,12 +294,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -309,43 +303,49 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -665,7 +665,7 @@
   <dimension ref="A2:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,523 +678,523 @@
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="13" t="s">
+      <c r="D3" s="24"/>
+      <c r="E3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="6" t="s">
+      <c r="F3" s="24"/>
+      <c r="G3" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="13" t="s">
+      <c r="H3" s="25"/>
+      <c r="I3" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="7"/>
-      <c r="K3" s="6" t="s">
+      <c r="J3" s="24"/>
+      <c r="K3" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="6"/>
-      <c r="M3" s="13" t="s">
+      <c r="L3" s="25"/>
+      <c r="M3" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="7"/>
+      <c r="N3" s="24"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="15" t="s">
+      <c r="J4" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="16" t="s">
+      <c r="K4" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="15" t="s">
+      <c r="L4" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="M4" s="14" t="s">
+      <c r="M4" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="N4" s="15" t="s">
+      <c r="N4" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="17">
-        <v>6.8235294117647101</v>
-      </c>
-      <c r="D5" s="18">
-        <v>0.51145606027038304</v>
-      </c>
-      <c r="E5" s="17">
-        <v>8.4705882352941195</v>
-      </c>
-      <c r="F5" s="18">
-        <v>0.48664709680156998</v>
-      </c>
-      <c r="G5" s="19">
-        <v>6.7058823529411802</v>
-      </c>
-      <c r="H5" s="19">
-        <v>0.39840953644479798</v>
-      </c>
-      <c r="I5" s="17">
-        <v>8</v>
-      </c>
-      <c r="J5" s="18">
-        <v>0.43057731639837399</v>
-      </c>
-      <c r="K5" s="19">
-        <v>8.625</v>
-      </c>
-      <c r="L5" s="19">
-        <v>0.41555319563052801</v>
-      </c>
-      <c r="M5" s="17">
-        <v>3</v>
-      </c>
-      <c r="N5" s="18">
-        <v>0.66904338246413197</v>
+      <c r="C5" s="14">
+        <v>6.34375</v>
+      </c>
+      <c r="D5" s="15">
+        <v>0.39556353991856102</v>
+      </c>
+      <c r="E5" s="14">
+        <v>7.9375</v>
+      </c>
+      <c r="F5" s="15">
+        <v>0.39639886030564297</v>
+      </c>
+      <c r="G5" s="16">
+        <v>7.09375</v>
+      </c>
+      <c r="H5" s="16">
+        <v>0.31863929133719698</v>
+      </c>
+      <c r="I5" s="14">
+        <v>7.84375</v>
+      </c>
+      <c r="J5" s="15">
+        <v>0.31143973359430299</v>
+      </c>
+      <c r="K5" s="16">
+        <v>8.32258064516129</v>
+      </c>
+      <c r="L5" s="16">
+        <v>0.42347029392505903</v>
+      </c>
+      <c r="M5" s="14">
+        <v>2.96875</v>
+      </c>
+      <c r="N5" s="15">
+        <v>0.46767349506238998</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="20">
-        <v>8.2352941176470598</v>
-      </c>
-      <c r="D6" s="21">
-        <v>0.58282290593501795</v>
-      </c>
-      <c r="E6" s="20">
-        <v>7.6470588235294104</v>
-      </c>
-      <c r="F6" s="21">
-        <v>0.53333333333333299</v>
-      </c>
-      <c r="G6" s="22">
-        <v>7.5882352941176503</v>
-      </c>
-      <c r="H6" s="22">
-        <v>0.33523268393901001</v>
-      </c>
-      <c r="I6" s="20">
-        <v>7.1176470588235299</v>
-      </c>
-      <c r="J6" s="21">
-        <v>0.472749472228223</v>
-      </c>
-      <c r="K6" s="22">
-        <v>7.4705882352941204</v>
-      </c>
-      <c r="L6" s="22">
-        <v>0.55947821496093397</v>
-      </c>
-      <c r="M6" s="20">
-        <v>2.1176470588235299</v>
-      </c>
-      <c r="N6" s="21">
-        <v>0.59361683970466395</v>
+      <c r="C6" s="17">
+        <v>8.3125</v>
+      </c>
+      <c r="D6" s="18">
+        <v>0.37145501833352801</v>
+      </c>
+      <c r="E6" s="17">
+        <v>7.1875</v>
+      </c>
+      <c r="F6" s="18">
+        <v>0.35762855798142201</v>
+      </c>
+      <c r="G6" s="19">
+        <v>7.765625</v>
+      </c>
+      <c r="H6" s="19">
+        <v>0.32764461763274799</v>
+      </c>
+      <c r="I6" s="17">
+        <v>6.9375</v>
+      </c>
+      <c r="J6" s="18">
+        <v>0.30432865034260997</v>
+      </c>
+      <c r="K6" s="19">
+        <v>6.5</v>
+      </c>
+      <c r="L6" s="19">
+        <v>0.466628262628691</v>
+      </c>
+      <c r="M6" s="17">
+        <v>1.59375</v>
+      </c>
+      <c r="N6" s="18">
+        <v>0.38326740170496798</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="20">
-        <v>9.7647058823529402</v>
-      </c>
-      <c r="D7" s="21">
-        <v>0.118187368057056</v>
-      </c>
-      <c r="E7" s="20">
-        <v>8.6176470588235308</v>
-      </c>
-      <c r="F7" s="21">
-        <v>0.26636888135137199</v>
-      </c>
-      <c r="G7" s="22">
-        <v>7.1764705882352899</v>
-      </c>
-      <c r="H7" s="22">
-        <v>0.47676156231557398</v>
-      </c>
-      <c r="I7" s="20">
-        <v>7.8823529411764701</v>
-      </c>
-      <c r="J7" s="21">
-        <v>0.35812563194215502</v>
-      </c>
-      <c r="K7" s="22">
-        <v>4.5294117647058796</v>
-      </c>
-      <c r="L7" s="22">
-        <v>0.54218839342820102</v>
-      </c>
-      <c r="M7" s="20">
-        <v>4.7058823529411802</v>
-      </c>
-      <c r="N7" s="21">
-        <v>0.752561762481463</v>
+      <c r="C7" s="17">
+        <v>9.625</v>
+      </c>
+      <c r="D7" s="18">
+        <v>0.22338127394297599</v>
+      </c>
+      <c r="E7" s="17">
+        <v>8.390625</v>
+      </c>
+      <c r="F7" s="18">
+        <v>0.227555353732002</v>
+      </c>
+      <c r="G7" s="19">
+        <v>6.84375</v>
+      </c>
+      <c r="H7" s="19">
+        <v>0.35670245744199902</v>
+      </c>
+      <c r="I7" s="17">
+        <v>8.03125</v>
+      </c>
+      <c r="J7" s="18">
+        <v>0.217594876414716</v>
+      </c>
+      <c r="K7" s="19">
+        <v>4.28125</v>
+      </c>
+      <c r="L7" s="19">
+        <v>0.40469615992104302</v>
+      </c>
+      <c r="M7" s="17">
+        <v>3.90625</v>
+      </c>
+      <c r="N7" s="18">
+        <v>0.51266101915838702</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="20">
-        <v>5.8235294117647101</v>
-      </c>
-      <c r="D8" s="21">
-        <v>0.65368309393894197</v>
-      </c>
-      <c r="E8" s="20">
-        <v>7.2941176470588198</v>
-      </c>
-      <c r="F8" s="21">
-        <v>0.69693205243717005</v>
-      </c>
-      <c r="G8" s="22">
-        <v>6.3529411764705896</v>
-      </c>
-      <c r="H8" s="22">
-        <v>0.60683932655520001</v>
-      </c>
-      <c r="I8" s="20">
-        <v>8.0588235294117592</v>
-      </c>
-      <c r="J8" s="21">
-        <v>0.42761798705987902</v>
-      </c>
-      <c r="K8" s="22">
-        <v>7.4705882352941204</v>
-      </c>
-      <c r="L8" s="22">
-        <v>0.62080337096122895</v>
-      </c>
-      <c r="M8" s="20">
-        <v>5.4117647058823497</v>
-      </c>
-      <c r="N8" s="21">
-        <v>1.02910039308496</v>
+      <c r="C8" s="17">
+        <v>5.6875</v>
+      </c>
+      <c r="D8" s="18">
+        <v>0.44999439960672799</v>
+      </c>
+      <c r="E8" s="17">
+        <v>7</v>
+      </c>
+      <c r="F8" s="18">
+        <v>0.52555654064939095</v>
+      </c>
+      <c r="G8" s="19">
+        <v>6.4375</v>
+      </c>
+      <c r="H8" s="19">
+        <v>0.34762297661542402</v>
+      </c>
+      <c r="I8" s="17">
+        <v>7.84375</v>
+      </c>
+      <c r="J8" s="18">
+        <v>0.42385846456555598</v>
+      </c>
+      <c r="K8" s="19">
+        <v>7.8125</v>
+      </c>
+      <c r="L8" s="19">
+        <v>0.42463812867261502</v>
+      </c>
+      <c r="M8" s="17">
+        <v>5.65625</v>
+      </c>
+      <c r="N8" s="18">
+        <v>0.66540276276368804</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="20">
-        <v>7.7941176470588198</v>
-      </c>
-      <c r="D9" s="21">
-        <v>0.447745676111105</v>
-      </c>
-      <c r="E9" s="20">
-        <v>9.8235294117647101</v>
-      </c>
-      <c r="F9" s="21">
-        <v>0.144749372891149</v>
-      </c>
-      <c r="G9" s="22">
-        <v>6.0625</v>
-      </c>
-      <c r="H9" s="22">
-        <v>0.39223227027636798</v>
-      </c>
-      <c r="I9" s="20">
-        <v>8.59375</v>
-      </c>
-      <c r="J9" s="21">
-        <v>0.48657406128097302</v>
-      </c>
-      <c r="K9" s="22">
-        <v>5.4375</v>
-      </c>
-      <c r="L9" s="22">
-        <v>0.48727931445760497</v>
-      </c>
-      <c r="M9" s="20">
-        <v>3.0588235294117601</v>
-      </c>
-      <c r="N9" s="21">
-        <v>0.76966288229389901</v>
+      <c r="C9" s="17">
+        <v>7.453125</v>
+      </c>
+      <c r="D9" s="18">
+        <v>0.33402434885049898</v>
+      </c>
+      <c r="E9" s="17">
+        <v>9.875</v>
+      </c>
+      <c r="F9" s="18">
+        <v>7.4460424647658799E-2</v>
+      </c>
+      <c r="G9" s="19">
+        <v>5.9354838709677402</v>
+      </c>
+      <c r="H9" s="19">
+        <v>0.37940384439521202</v>
+      </c>
+      <c r="I9" s="17">
+        <v>8.7258064516129004</v>
+      </c>
+      <c r="J9" s="18">
+        <v>0.278087467555652</v>
+      </c>
+      <c r="K9" s="19">
+        <v>5.1612903225806503</v>
+      </c>
+      <c r="L9" s="19">
+        <v>0.40453550741599797</v>
+      </c>
+      <c r="M9" s="17">
+        <v>2.875</v>
+      </c>
+      <c r="N9" s="18">
+        <v>0.46608787071302998</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="20">
-        <v>7.8235294117647101</v>
-      </c>
-      <c r="D10" s="21">
-        <v>0</v>
-      </c>
-      <c r="E10" s="20">
-        <v>7.8823529411764701</v>
-      </c>
-      <c r="F10" s="21">
-        <v>0.52553827281224397</v>
-      </c>
-      <c r="G10" s="22">
-        <v>7</v>
-      </c>
-      <c r="H10" s="22">
-        <v>0.55947821496093397</v>
-      </c>
-      <c r="I10" s="20">
-        <v>6.8235294117647101</v>
-      </c>
-      <c r="J10" s="21">
-        <v>0.613084835787851</v>
-      </c>
-      <c r="K10" s="22">
-        <v>8.2941176470588207</v>
-      </c>
-      <c r="L10" s="22">
-        <v>0.58118652580542296</v>
-      </c>
-      <c r="M10" s="20">
-        <v>1.70588235294118</v>
-      </c>
-      <c r="N10" s="21">
-        <v>0.51823877563477305</v>
+      <c r="C10" s="17">
+        <v>7.34375</v>
+      </c>
+      <c r="D10" s="18">
+        <v>0.36920079061443301</v>
+      </c>
+      <c r="E10" s="17">
+        <v>8.125</v>
+      </c>
+      <c r="F10" s="18">
+        <v>0.366846852110286</v>
+      </c>
+      <c r="G10" s="19">
+        <v>7.375</v>
+      </c>
+      <c r="H10" s="19">
+        <v>0.43009282568961499</v>
+      </c>
+      <c r="I10" s="17">
+        <v>7.625</v>
+      </c>
+      <c r="J10" s="18">
+        <v>0.35568539016129602</v>
+      </c>
+      <c r="K10" s="19">
+        <v>7.28125</v>
+      </c>
+      <c r="L10" s="19">
+        <v>0.47780237639331302</v>
+      </c>
+      <c r="M10" s="17">
+        <v>1.34375</v>
+      </c>
+      <c r="N10" s="18">
+        <v>0.33181251689917901</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="20">
-        <v>7.8235294117647101</v>
-      </c>
-      <c r="D11" s="21">
-        <v>0.62488094104092395</v>
-      </c>
-      <c r="E11" s="20">
-        <v>6.4705882352941204</v>
-      </c>
-      <c r="F11" s="21">
-        <v>0.336178335137577</v>
-      </c>
-      <c r="G11" s="22">
-        <v>8.6764705882352899</v>
-      </c>
-      <c r="H11" s="22">
-        <v>0.38688827803713599</v>
-      </c>
-      <c r="I11" s="20">
-        <v>7.5882352941176503</v>
-      </c>
-      <c r="J11" s="21">
-        <v>0.350056684752173</v>
-      </c>
-      <c r="K11" s="22">
-        <v>8.1764705882352899</v>
-      </c>
-      <c r="L11" s="22">
-        <v>0.48271717704663503</v>
-      </c>
-      <c r="M11" s="20">
-        <v>2.1176470588235299</v>
-      </c>
-      <c r="N11" s="21">
-        <v>0.53866383780492499</v>
+      <c r="C11" s="17">
+        <v>8.0625</v>
+      </c>
+      <c r="D11" s="18">
+        <v>0.403955992093677</v>
+      </c>
+      <c r="E11" s="17">
+        <v>6.8125</v>
+      </c>
+      <c r="F11" s="18">
+        <v>0.35762855798142201</v>
+      </c>
+      <c r="G11" s="19">
+        <v>8.578125</v>
+      </c>
+      <c r="H11" s="19">
+        <v>0.30709796610575302</v>
+      </c>
+      <c r="I11" s="17">
+        <v>7.640625</v>
+      </c>
+      <c r="J11" s="18">
+        <v>0.32084375201279097</v>
+      </c>
+      <c r="K11" s="19">
+        <v>6.96875</v>
+      </c>
+      <c r="L11" s="19">
+        <v>0.46551301695184999</v>
+      </c>
+      <c r="M11" s="17">
+        <v>1.9375</v>
+      </c>
+      <c r="N11" s="18">
+        <v>0.38083498034984198</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="20">
-        <v>4.2941176470588198</v>
-      </c>
-      <c r="D12" s="21">
-        <v>0.64880843162861301</v>
-      </c>
-      <c r="E12" s="20">
-        <v>5.1764705882352899</v>
-      </c>
-      <c r="F12" s="21">
-        <v>0.44149817091425803</v>
-      </c>
-      <c r="G12" s="22">
-        <v>7</v>
-      </c>
-      <c r="H12" s="22">
-        <v>0.39036002917941298</v>
-      </c>
-      <c r="I12" s="20">
-        <v>7.5882352941176503</v>
-      </c>
-      <c r="J12" s="21">
-        <v>0.306542417893925</v>
-      </c>
-      <c r="K12" s="22">
-        <v>7.5441176470588198</v>
-      </c>
-      <c r="L12" s="22">
-        <v>0.46598589800857398</v>
-      </c>
-      <c r="M12" s="20">
-        <v>10</v>
-      </c>
-      <c r="N12" s="21">
-        <v>0</v>
+      <c r="C12" s="17">
+        <v>4.03125</v>
+      </c>
+      <c r="D12" s="18">
+        <v>0.42711611466113703</v>
+      </c>
+      <c r="E12" s="17">
+        <v>4.65625</v>
+      </c>
+      <c r="F12" s="18">
+        <v>0.41056946830768098</v>
+      </c>
+      <c r="G12" s="19">
+        <v>6.84375</v>
+      </c>
+      <c r="H12" s="19">
+        <v>0.25836557854601899</v>
+      </c>
+      <c r="I12" s="17">
+        <v>7.625</v>
+      </c>
+      <c r="J12" s="18">
+        <v>0.209405841493529</v>
+      </c>
+      <c r="K12" s="19">
+        <v>7.1796875</v>
+      </c>
+      <c r="L12" s="19">
+        <v>0.43681316694616701</v>
+      </c>
+      <c r="M12" s="17">
+        <v>9.90625</v>
+      </c>
+      <c r="N12" s="18">
+        <v>9.375E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="20">
-        <v>5.3529411764705896</v>
-      </c>
-      <c r="D13" s="21">
-        <v>0.61618385217606897</v>
-      </c>
-      <c r="E13" s="20">
-        <v>4.9411764705882399</v>
-      </c>
-      <c r="F13" s="21">
-        <v>0.45215533220835102</v>
-      </c>
-      <c r="G13" s="22">
-        <v>6.5882352941176503</v>
-      </c>
-      <c r="H13" s="22">
-        <v>0.51145606027038304</v>
-      </c>
-      <c r="I13" s="20">
-        <v>7.2647058823529402</v>
-      </c>
-      <c r="J13" s="21">
-        <v>0.447745676111105</v>
-      </c>
-      <c r="K13" s="22">
-        <v>6.6764705882352899</v>
-      </c>
-      <c r="L13" s="22">
-        <v>0.70668575895143204</v>
-      </c>
-      <c r="M13" s="20">
-        <v>9.2352941176470598</v>
-      </c>
-      <c r="N13" s="21">
-        <v>0.55606326007600004</v>
+      <c r="C13" s="17">
+        <v>5.46875</v>
+      </c>
+      <c r="D13" s="18">
+        <v>0.462253367108587</v>
+      </c>
+      <c r="E13" s="17">
+        <v>5.03125</v>
+      </c>
+      <c r="F13" s="18">
+        <v>0.32217874409271802</v>
+      </c>
+      <c r="G13" s="19">
+        <v>6.53125</v>
+      </c>
+      <c r="H13" s="19">
+        <v>0.39905224160786001</v>
+      </c>
+      <c r="I13" s="17">
+        <v>6.921875</v>
+      </c>
+      <c r="J13" s="18">
+        <v>0.32387318228844603</v>
+      </c>
+      <c r="K13" s="19">
+        <v>6.5625</v>
+      </c>
+      <c r="L13" s="19">
+        <v>0.45873027776890402</v>
+      </c>
+      <c r="M13" s="17">
+        <v>9.09375</v>
+      </c>
+      <c r="N13" s="18">
+        <v>0.38195004476180999</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="23">
-        <v>7</v>
-      </c>
-      <c r="D14" s="24">
-        <v>2.3577157439801302</v>
-      </c>
-      <c r="E14" s="23">
-        <v>9</v>
-      </c>
-      <c r="F14" s="24">
-        <v>2.5724787771376301</v>
-      </c>
-      <c r="G14" s="25">
-        <v>5</v>
-      </c>
-      <c r="H14" s="25">
-        <v>2.0651164331225802</v>
-      </c>
-      <c r="I14" s="23">
-        <v>12</v>
-      </c>
-      <c r="J14" s="24">
-        <v>2.7865221840769401</v>
-      </c>
-      <c r="K14" s="25">
+      <c r="C14" s="20">
+        <v>15</v>
+      </c>
+      <c r="D14" s="21">
+        <v>3.4396200248709099</v>
+      </c>
+      <c r="E14" s="20">
+        <v>21</v>
+      </c>
+      <c r="F14" s="21">
+        <v>3.8456120961904299</v>
+      </c>
+      <c r="G14" s="22">
+        <v>11</v>
+      </c>
+      <c r="H14" s="22">
+        <v>3.0488972839187798</v>
+      </c>
+      <c r="I14" s="20">
+        <v>23</v>
+      </c>
+      <c r="J14" s="21">
+        <v>3.9432595368106198</v>
+      </c>
+      <c r="K14" s="22">
         <v>0</v>
       </c>
-      <c r="L14" s="25">
+      <c r="L14" s="22">
         <v>0</v>
       </c>
-      <c r="M14" s="23">
+      <c r="M14" s="20">
         <v>1</v>
       </c>
-      <c r="N14" s="24">
-        <v>0.98518436614377802</v>
+      <c r="N14" s="21">
+        <v>0.99293277363462396</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="M3:N3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>